<commit_message>
[add] - add function export AC long and short term
</commit_message>
<xml_diff>
--- a/MANAGER/Content/assets/excel/Collaboration/Download/Partner.xlsx
+++ b/MANAGER/Content/assets/excel/Collaboration/Download/Partner.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="202">
   <si>
     <t>STT</t>
   </si>
@@ -57,6 +57,90 @@
     <t>Địa chỉ</t>
   </si>
   <si>
+    <t>Deakin University</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t xml:space="preserve">Công nghệ thông tin, _x000D_Khoa học tự nhiên</t>
+  </si>
+  <si>
+    <t>Đã có</t>
+  </si>
+  <si>
+    <t>James Cook University</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Công nghệ thông tin, _x000D_Khoa học xã hội</t>
+  </si>
+  <si>
+    <t>Macquarie University</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Công nghệ thông tin, _x000D_Ngôn ngữ</t>
+  </si>
+  <si>
+    <t>Queensland University of Technology</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1vi1sttkutztyofujf6d1wmuvs2jaxh2c</t>
+  </si>
+  <si>
+    <t>Công nghệ thông tin</t>
+  </si>
+  <si>
+    <t>Swinburne University of Technology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://drive.google.com/drive/folders/1tuqwluvlbka_vzcgkdj2olrqtfnrjqxv_x000D_
+_x000D_
+</t>
+  </si>
+  <si>
+    <t>University of Technology Sydney</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://drive.google.com/drive/u/0/folders/1ywq6-h8okh-jcuclrgymvxg-z-q978j__x000D_
+</t>
+  </si>
+  <si>
+    <t>Euro Education Fair</t>
+  </si>
+  <si>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Khoa học tự nhiên, _x000D_Khoa học xã hội</t>
+  </si>
+  <si>
+    <t>Fair International</t>
+  </si>
+  <si>
+    <t>Glee Education</t>
+  </si>
+  <si>
+    <t>Global Immigration Consultants Ltd.</t>
+  </si>
+  <si>
+    <t>https://www.ue.edu.ph/manila/main.html?page=students&amp;link=iso</t>
+  </si>
+  <si>
+    <t>Greybites Consultlants</t>
+  </si>
+  <si>
+    <t>Artevelde University College Ghent</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Khoa học xã hội, _x000D_Ngôn ngữ</t>
+  </si>
+  <si>
     <t>National Institute of Posts, Telecommunications and ICT</t>
   </si>
   <si>
@@ -67,6 +151,9 @@
   </si>
   <si>
     <t>Plus Enterprises Co., Ltd. (t/a: plus education)</t>
+  </si>
+  <si>
+    <t>Zaman University</t>
   </si>
   <si>
     <t>Alpha Consultancy Agency Ltd.</t>
@@ -280,6 +367,19 @@
     <t>Kindai University</t>
   </si>
   <si>
+    <t xml:space="preserve">Kyoto Computer Gakuin_x000D_
+ - The Kyoto College of Graduate Studies for Information</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1qjyjdgmbgkmrftj6n-0cpynrsewytwkz</t>
+  </si>
+  <si>
+    <t>Kyoto University of Foreign Studies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kinh tế - quản lý, _x000D_Ngôn ngữ</t>
+  </si>
+  <si>
     <t>Kyushu Institute of Technology</t>
   </si>
   <si>
@@ -346,6 +446,13 @@
     <t>https://drive.google.com/drive/folders/1oajpj6a6iw65a-bk049l0mytajlw4vsz</t>
   </si>
   <si>
+    <t>Universiti Teknologi Petronas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://drive.google.com/drive/folders/1p876oqt_paeysyfj974yrojfxo0drk91_x000D_
+</t>
+  </si>
+  <si>
     <t>University College Technology Sarawak</t>
   </si>
   <si>
@@ -518,6 +625,27 @@
   </si>
   <si>
     <t>United States of America (the)</t>
+  </si>
+  <si>
+    <t>Universiti Brunei Darussalam</t>
+  </si>
+  <si>
+    <t>Brunei Darussalam</t>
+  </si>
+  <si>
+    <t>http://www.ubd.edu.bn/menu/service-and-administration/student-affairs-section/international-student-office/</t>
+  </si>
+  <si>
+    <t>Universiti Teknologi Brunei</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/12iEPuJzmk6Ausqjz8aOZJyrFoY1hDto5</t>
+  </si>
+  <si>
+    <t>Ural Federal University</t>
+  </si>
+  <si>
+    <t>Russian Federation (the)</t>
   </si>
 </sst>
 </file>
@@ -884,7 +1012,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E9AC343-7D93-44F6-8344-984448AAB95C}">
-  <dimension ref="A1:G106"/>
+  <dimension ref="A1:G125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F1" activeCellId="3" sqref="A1:A1048576 C1:C1048576 E1:E1048576 F1:F1048576"/>
@@ -926,7 +1054,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>7</v>
@@ -934,1641 +1062,1994 @@
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="D2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F3" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="F5" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="F6" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="F7" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="F8" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="F9" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="F10" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F11" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="F12" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="F13" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="F16" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>38</v>
+        <v>44</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>45</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>38</v>
+        <v>52</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>51</v>
+        <v>66</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>69</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D38" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="B41" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>67</v>
+        <v>88</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>89</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>67</v>
+        <v>88</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>91</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D54" s="0" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>67</v>
+        <v>95</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>97</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>67</v>
+        <v>95</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>99</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D57" s="0" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="2">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D61" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="2">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="2">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="2">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="B64" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="2">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="E65" s="2"/>
       <c r="F65" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="2">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E66" s="2"/>
+        <v>95</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="F66" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="2">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E67" s="2"/>
+        <v>95</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="F67" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="2">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E68" s="2"/>
       <c r="F68" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="2">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="E69" s="2"/>
       <c r="F69" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="2">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E70" s="2"/>
       <c r="F70" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="2">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="2">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="E72" s="2"/>
       <c r="F72" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="2">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D73" s="0" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="E73" s="2"/>
       <c r="F73" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="2">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D74" s="0" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="E74" s="2"/>
       <c r="F74" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="2">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D75" s="0" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="E75" s="2"/>
       <c r="F75" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="2">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>115</v>
+        <v>95</v>
+      </c>
+      <c r="D76" s="0" t="s">
+        <v>124</v>
       </c>
       <c r="E76" s="2"/>
       <c r="F76" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="2">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="E77" s="2"/>
       <c r="F77" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="2">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="E78" s="2"/>
       <c r="F78" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="2">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="E79" s="2"/>
       <c r="F79" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="2">
+        <v>79</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="B80" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="E80" s="2"/>
       <c r="F80" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="2">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E81" s="2"/>
       <c r="F81" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="2">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E82" s="2"/>
       <c r="F82" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="2">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E83" s="2"/>
       <c r="F83" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="2">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>120</v>
+        <v>130</v>
+      </c>
+      <c r="D84" s="0" t="s">
+        <v>134</v>
       </c>
       <c r="E84" s="2"/>
       <c r="F84" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="2">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E85" s="2"/>
+        <v>130</v>
+      </c>
+      <c r="D85" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="F85" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="2">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="E86" s="2"/>
       <c r="F86" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="2">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D87" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E87" s="2"/>
       <c r="F87" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="2">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>126</v>
+        <v>140</v>
+      </c>
+      <c r="D88" s="0" t="s">
+        <v>141</v>
       </c>
       <c r="E88" s="2"/>
       <c r="F88" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="2">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="E89" s="2"/>
       <c r="F89" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="2">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>132</v>
+        <v>140</v>
+      </c>
+      <c r="D90" s="0" t="s">
+        <v>145</v>
       </c>
       <c r="E90" s="2"/>
       <c r="F90" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="2">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>132</v>
+        <v>140</v>
+      </c>
+      <c r="D91" s="0" t="s">
+        <v>147</v>
       </c>
       <c r="E91" s="2"/>
       <c r="F91" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="2">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="E92" s="2"/>
       <c r="F92" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="2">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D93" s="0" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="E93" s="2"/>
       <c r="F93" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="2">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="D94" s="0" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="E94" s="2"/>
       <c r="F94" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="2">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="E95" s="2"/>
       <c r="F95" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="2">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="E96" s="2"/>
       <c r="F96" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="2">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="E97" s="2"/>
       <c r="F97" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="2">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D98" s="0" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="E98" s="2"/>
       <c r="F98" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="2">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="E99" s="2"/>
       <c r="F99" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="2">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="E100" s="2"/>
       <c r="F100" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="2">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D101" s="0" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="E101" s="2"/>
       <c r="F101" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="2">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D102" s="0" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="E102" s="2"/>
       <c r="F102" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="2">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>145</v>
+        <v>160</v>
+      </c>
+      <c r="D103" s="0" t="s">
+        <v>163</v>
       </c>
       <c r="E103" s="2"/>
       <c r="F103" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="2">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="E104" s="2"/>
       <c r="F104" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="2">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="D105" s="0" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="E105" s="2"/>
       <c r="F105" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="2">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="E106" s="2"/>
       <c r="F106" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="2">
+        <v>106</v>
+      </c>
+      <c r="B107" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E107" s="2"/>
+      <c r="F107" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="2">
+        <v>107</v>
+      </c>
+      <c r="B108" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E108" s="2"/>
+      <c r="F108" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="2">
+        <v>108</v>
+      </c>
+      <c r="B109" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D109" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="E109" s="2"/>
+      <c r="F109" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="2">
+        <v>109</v>
+      </c>
+      <c r="B110" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D110" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="E110" s="2"/>
+      <c r="F110" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="2">
+        <v>110</v>
+      </c>
+      <c r="B111" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E111" s="2"/>
+      <c r="F111" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="2">
+        <v>111</v>
+      </c>
+      <c r="B112" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E112" s="2"/>
+      <c r="F112" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="2">
+        <v>112</v>
+      </c>
+      <c r="B113" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E113" s="2"/>
+      <c r="F113" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="2">
+        <v>113</v>
+      </c>
+      <c r="B114" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D114" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="E114" s="2"/>
+      <c r="F114" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="2">
+        <v>114</v>
+      </c>
+      <c r="B115" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E115" s="2"/>
+      <c r="F115" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="2">
+        <v>115</v>
+      </c>
+      <c r="B116" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E116" s="2"/>
+      <c r="F116" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="2">
+        <v>116</v>
+      </c>
+      <c r="B117" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D117" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="E117" s="2"/>
+      <c r="F117" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="2">
+        <v>117</v>
+      </c>
+      <c r="B118" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D118" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="E118" s="2"/>
+      <c r="F118" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="2">
+        <v>118</v>
+      </c>
+      <c r="B119" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E119" s="2"/>
+      <c r="F119" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="2">
+        <v>119</v>
+      </c>
+      <c r="B120" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E120" s="2"/>
+      <c r="F120" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="2">
+        <v>120</v>
+      </c>
+      <c r="B121" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D121" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="E121" s="2"/>
+      <c r="F121" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="2">
+        <v>121</v>
+      </c>
+      <c r="B122" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E122" s="2"/>
+      <c r="F122" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="2">
+        <v>122</v>
+      </c>
+      <c r="B123" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D123" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="2">
+        <v>123</v>
+      </c>
+      <c r="B124" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D124" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="2">
+        <v>124</v>
+      </c>
+      <c r="B125" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[add] - add function export AC long and short term (#1063)
</commit_message>
<xml_diff>
--- a/MANAGER/Content/assets/excel/Collaboration/Download/Partner.xlsx
+++ b/MANAGER/Content/assets/excel/Collaboration/Download/Partner.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="202">
   <si>
     <t>STT</t>
   </si>
@@ -57,6 +57,90 @@
     <t>Địa chỉ</t>
   </si>
   <si>
+    <t>Deakin University</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t xml:space="preserve">Công nghệ thông tin, _x000D_Khoa học tự nhiên</t>
+  </si>
+  <si>
+    <t>Đã có</t>
+  </si>
+  <si>
+    <t>James Cook University</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Công nghệ thông tin, _x000D_Khoa học xã hội</t>
+  </si>
+  <si>
+    <t>Macquarie University</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Công nghệ thông tin, _x000D_Ngôn ngữ</t>
+  </si>
+  <si>
+    <t>Queensland University of Technology</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1vi1sttkutztyofujf6d1wmuvs2jaxh2c</t>
+  </si>
+  <si>
+    <t>Công nghệ thông tin</t>
+  </si>
+  <si>
+    <t>Swinburne University of Technology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://drive.google.com/drive/folders/1tuqwluvlbka_vzcgkdj2olrqtfnrjqxv_x000D_
+_x000D_
+</t>
+  </si>
+  <si>
+    <t>University of Technology Sydney</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://drive.google.com/drive/u/0/folders/1ywq6-h8okh-jcuclrgymvxg-z-q978j__x000D_
+</t>
+  </si>
+  <si>
+    <t>Euro Education Fair</t>
+  </si>
+  <si>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Khoa học tự nhiên, _x000D_Khoa học xã hội</t>
+  </si>
+  <si>
+    <t>Fair International</t>
+  </si>
+  <si>
+    <t>Glee Education</t>
+  </si>
+  <si>
+    <t>Global Immigration Consultants Ltd.</t>
+  </si>
+  <si>
+    <t>https://www.ue.edu.ph/manila/main.html?page=students&amp;link=iso</t>
+  </si>
+  <si>
+    <t>Greybites Consultlants</t>
+  </si>
+  <si>
+    <t>Artevelde University College Ghent</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Khoa học xã hội, _x000D_Ngôn ngữ</t>
+  </si>
+  <si>
     <t>National Institute of Posts, Telecommunications and ICT</t>
   </si>
   <si>
@@ -67,6 +151,9 @@
   </si>
   <si>
     <t>Plus Enterprises Co., Ltd. (t/a: plus education)</t>
+  </si>
+  <si>
+    <t>Zaman University</t>
   </si>
   <si>
     <t>Alpha Consultancy Agency Ltd.</t>
@@ -280,6 +367,19 @@
     <t>Kindai University</t>
   </si>
   <si>
+    <t xml:space="preserve">Kyoto Computer Gakuin_x000D_
+ - The Kyoto College of Graduate Studies for Information</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1qjyjdgmbgkmrftj6n-0cpynrsewytwkz</t>
+  </si>
+  <si>
+    <t>Kyoto University of Foreign Studies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kinh tế - quản lý, _x000D_Ngôn ngữ</t>
+  </si>
+  <si>
     <t>Kyushu Institute of Technology</t>
   </si>
   <si>
@@ -346,6 +446,13 @@
     <t>https://drive.google.com/drive/folders/1oajpj6a6iw65a-bk049l0mytajlw4vsz</t>
   </si>
   <si>
+    <t>Universiti Teknologi Petronas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://drive.google.com/drive/folders/1p876oqt_paeysyfj974yrojfxo0drk91_x000D_
+</t>
+  </si>
+  <si>
     <t>University College Technology Sarawak</t>
   </si>
   <si>
@@ -518,6 +625,27 @@
   </si>
   <si>
     <t>United States of America (the)</t>
+  </si>
+  <si>
+    <t>Universiti Brunei Darussalam</t>
+  </si>
+  <si>
+    <t>Brunei Darussalam</t>
+  </si>
+  <si>
+    <t>http://www.ubd.edu.bn/menu/service-and-administration/student-affairs-section/international-student-office/</t>
+  </si>
+  <si>
+    <t>Universiti Teknologi Brunei</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/12iEPuJzmk6Ausqjz8aOZJyrFoY1hDto5</t>
+  </si>
+  <si>
+    <t>Ural Federal University</t>
+  </si>
+  <si>
+    <t>Russian Federation (the)</t>
   </si>
 </sst>
 </file>
@@ -884,7 +1012,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E9AC343-7D93-44F6-8344-984448AAB95C}">
-  <dimension ref="A1:G106"/>
+  <dimension ref="A1:G125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F1" activeCellId="3" sqref="A1:A1048576 C1:C1048576 E1:E1048576 F1:F1048576"/>
@@ -926,7 +1054,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>7</v>
@@ -934,1641 +1062,1994 @@
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="D2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F3" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="F5" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="F6" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="F7" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="F8" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="F9" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="F10" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F11" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="F12" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="F13" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="F16" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>38</v>
+        <v>44</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>45</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>38</v>
+        <v>52</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>51</v>
+        <v>66</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>69</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D38" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="B41" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>67</v>
+        <v>88</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>89</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>67</v>
+        <v>88</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>91</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D54" s="0" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>67</v>
+        <v>95</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>97</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>67</v>
+        <v>95</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>99</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D57" s="0" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="2">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D61" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="2">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="2">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="2">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="B64" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="2">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="E65" s="2"/>
       <c r="F65" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="2">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E66" s="2"/>
+        <v>95</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="F66" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="2">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E67" s="2"/>
+        <v>95</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="F67" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="2">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E68" s="2"/>
       <c r="F68" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="2">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="E69" s="2"/>
       <c r="F69" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="2">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E70" s="2"/>
       <c r="F70" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="2">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="2">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="E72" s="2"/>
       <c r="F72" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="2">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D73" s="0" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="E73" s="2"/>
       <c r="F73" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="2">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D74" s="0" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="E74" s="2"/>
       <c r="F74" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="2">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D75" s="0" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="E75" s="2"/>
       <c r="F75" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="2">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>115</v>
+        <v>95</v>
+      </c>
+      <c r="D76" s="0" t="s">
+        <v>124</v>
       </c>
       <c r="E76" s="2"/>
       <c r="F76" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="2">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="E77" s="2"/>
       <c r="F77" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="2">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="E78" s="2"/>
       <c r="F78" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="2">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="E79" s="2"/>
       <c r="F79" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="2">
+        <v>79</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="B80" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="E80" s="2"/>
       <c r="F80" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="2">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E81" s="2"/>
       <c r="F81" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="2">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E82" s="2"/>
       <c r="F82" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="2">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E83" s="2"/>
       <c r="F83" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="2">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>120</v>
+        <v>130</v>
+      </c>
+      <c r="D84" s="0" t="s">
+        <v>134</v>
       </c>
       <c r="E84" s="2"/>
       <c r="F84" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="2">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E85" s="2"/>
+        <v>130</v>
+      </c>
+      <c r="D85" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="F85" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="2">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="E86" s="2"/>
       <c r="F86" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="2">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D87" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E87" s="2"/>
       <c r="F87" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="2">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>126</v>
+        <v>140</v>
+      </c>
+      <c r="D88" s="0" t="s">
+        <v>141</v>
       </c>
       <c r="E88" s="2"/>
       <c r="F88" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="2">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="E89" s="2"/>
       <c r="F89" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="2">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>132</v>
+        <v>140</v>
+      </c>
+      <c r="D90" s="0" t="s">
+        <v>145</v>
       </c>
       <c r="E90" s="2"/>
       <c r="F90" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="2">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>132</v>
+        <v>140</v>
+      </c>
+      <c r="D91" s="0" t="s">
+        <v>147</v>
       </c>
       <c r="E91" s="2"/>
       <c r="F91" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="2">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="E92" s="2"/>
       <c r="F92" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="2">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D93" s="0" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="E93" s="2"/>
       <c r="F93" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="2">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="D94" s="0" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="E94" s="2"/>
       <c r="F94" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="2">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="E95" s="2"/>
       <c r="F95" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="2">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="E96" s="2"/>
       <c r="F96" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="2">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="E97" s="2"/>
       <c r="F97" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="2">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D98" s="0" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="E98" s="2"/>
       <c r="F98" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="2">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="E99" s="2"/>
       <c r="F99" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="2">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="E100" s="2"/>
       <c r="F100" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="2">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D101" s="0" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="E101" s="2"/>
       <c r="F101" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="2">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D102" s="0" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="E102" s="2"/>
       <c r="F102" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="2">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>145</v>
+        <v>160</v>
+      </c>
+      <c r="D103" s="0" t="s">
+        <v>163</v>
       </c>
       <c r="E103" s="2"/>
       <c r="F103" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="2">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="E104" s="2"/>
       <c r="F104" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="2">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="D105" s="0" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="E105" s="2"/>
       <c r="F105" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="2">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="E106" s="2"/>
       <c r="F106" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="2">
+        <v>106</v>
+      </c>
+      <c r="B107" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E107" s="2"/>
+      <c r="F107" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="2">
+        <v>107</v>
+      </c>
+      <c r="B108" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E108" s="2"/>
+      <c r="F108" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="2">
+        <v>108</v>
+      </c>
+      <c r="B109" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D109" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="E109" s="2"/>
+      <c r="F109" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="2">
+        <v>109</v>
+      </c>
+      <c r="B110" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D110" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="E110" s="2"/>
+      <c r="F110" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="2">
+        <v>110</v>
+      </c>
+      <c r="B111" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E111" s="2"/>
+      <c r="F111" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="2">
+        <v>111</v>
+      </c>
+      <c r="B112" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E112" s="2"/>
+      <c r="F112" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="2">
+        <v>112</v>
+      </c>
+      <c r="B113" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E113" s="2"/>
+      <c r="F113" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="2">
+        <v>113</v>
+      </c>
+      <c r="B114" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D114" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="E114" s="2"/>
+      <c r="F114" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="2">
+        <v>114</v>
+      </c>
+      <c r="B115" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E115" s="2"/>
+      <c r="F115" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="2">
+        <v>115</v>
+      </c>
+      <c r="B116" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E116" s="2"/>
+      <c r="F116" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="2">
+        <v>116</v>
+      </c>
+      <c r="B117" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D117" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="E117" s="2"/>
+      <c r="F117" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="2">
+        <v>117</v>
+      </c>
+      <c r="B118" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D118" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="E118" s="2"/>
+      <c r="F118" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="2">
+        <v>118</v>
+      </c>
+      <c r="B119" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E119" s="2"/>
+      <c r="F119" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="2">
+        <v>119</v>
+      </c>
+      <c r="B120" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E120" s="2"/>
+      <c r="F120" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="2">
+        <v>120</v>
+      </c>
+      <c r="B121" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D121" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="E121" s="2"/>
+      <c r="F121" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="2">
+        <v>121</v>
+      </c>
+      <c r="B122" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E122" s="2"/>
+      <c r="F122" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="2">
+        <v>122</v>
+      </c>
+      <c r="B123" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D123" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="2">
+        <v>123</v>
+      </c>
+      <c r="B124" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D124" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="2">
+        <v>124</v>
+      </c>
+      <c r="B125" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>